<commit_message>
Preventive + Sensitivity Analysis Prognostics
</commit_message>
<xml_diff>
--- a/PxM_PPC_RL/visuals/Analysis.xlsx
+++ b/PxM_PPC_RL/visuals/Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w_kevi02\sciebo\PhD\01 Prescriptive Maintenance\30 RQ3 - Digital Twin\PxM &amp; PPC (R)\RL-PxM\PxM_PPC_RL\visuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1753B8-184D-4555-93A9-593FA1C869D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB95A6AB-F4C4-4407-8175-ED80AEF2111C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -73,30 +73,12 @@
     <t>DQN</t>
   </si>
   <si>
-    <t>PPO_DIAG_model.zip; PPO_ID_lookup_data.xlsx; tsne.html; tsne_files; PPO_raw_data.xlsx; PPO_rollout_ep_rew_mean.csv; PPO_state_action.xlsx; tensorboard/PPO_DIAG_model_2</t>
-  </si>
-  <si>
-    <t>tensorboard\DQN_REACT_model_3; best_DQN_reactive.zip</t>
-  </si>
-  <si>
-    <t>DQN_ID_lookup_data.xlsx; DQN_raw_data.xlsx; DQN_rollout_ep_rew_mean.csv; DQN_state_action.xlsx</t>
-  </si>
-  <si>
-    <t>best_A2C_predhealth.zip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A2C_rollout_ep_rew_mean.csv; A2C_DIAG_model.zip; best_A2C_2_predhealth.zip; tensorboard/A2C_DIAG_model_4 </t>
-  </si>
-  <si>
     <t>A2C_2</t>
   </si>
   <si>
     <t>Reactive</t>
   </si>
   <si>
-    <t>best_PPO_reactive.zip</t>
-  </si>
-  <si>
     <t>True Health</t>
   </si>
   <si>
@@ -112,17 +94,80 @@
     <t xml:space="preserve">True Health, gamma = 0.99, learning_rate=0.01 </t>
   </si>
   <si>
-    <t>best_DQN_truehealth.zip</t>
-  </si>
-  <si>
-    <t>best_PPO_truehealth.zip</t>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>9.zip;  tensorboard\9</t>
+  </si>
+  <si>
+    <t>Reactive, w/o condition/health knowledge</t>
+  </si>
+  <si>
+    <t>6_rew.csv; 6.zip; tensorboard/6</t>
+  </si>
+  <si>
+    <t>8.zip</t>
+  </si>
+  <si>
+    <t>7.zip</t>
+  </si>
+  <si>
+    <t>tensorboard\5; 5.zip</t>
+  </si>
+  <si>
+    <t>3.zip</t>
+  </si>
+  <si>
+    <t>4_ID.xlsx; tsne.html; tsne_files; 4_raw.xlsx; 4_rew.csv; 4_state_action.xlsx; tensorboard/4</t>
+  </si>
+  <si>
+    <t>2_ID.xlsx; 2_raw.xlsx; 2_rew.csv; 2_state_action.xlsx</t>
+  </si>
+  <si>
+    <t>1.zip</t>
+  </si>
+  <si>
+    <t>tensorboard\10; 10.zip</t>
+  </si>
+  <si>
+    <t>Reactive, gamma = 0.99, learning_rate=0.01, w/o condition/health knowledge</t>
+  </si>
+  <si>
+    <t>tensorboard\11; 11.zip</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Reactive, simple produce = order heuristic (action = obs[0]), MTBF = 22.352</t>
+  </si>
+  <si>
+    <t>Scheduled heuristic, MTBF = 22.352, MTBF*0.9-1: action = order + spare part, MTBF*0.9: action = maintain, else: action = order</t>
+  </si>
+  <si>
+    <t>Scheduled heuristic, MTBF = 22.352, MTBF*0.85-1: action = order + spare part, MTBF*0.85: action = maintain, else: action = order</t>
+  </si>
+  <si>
+    <t>Prognostics with exponential intensity</t>
+  </si>
+  <si>
+    <t>Training Time</t>
+  </si>
+  <si>
+    <t>06:34:35.6</t>
+  </si>
+  <si>
+    <t>tensorboard\15; 15.zip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,6 +179,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,10 +216,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -449,283 +506,522 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="10" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="12" width="73.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44655</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>0.01</v>
+      </c>
+      <c r="G2">
+        <v>3.99</v>
+      </c>
+      <c r="H2">
+        <v>1.34</v>
+      </c>
+      <c r="I2">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="J2">
+        <v>487</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44706</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>0.34</v>
+      </c>
+      <c r="G3">
+        <v>3.67</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>6.99</v>
+      </c>
+      <c r="J3">
+        <v>313</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44714</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>4.01</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>177</v>
+      </c>
+      <c r="I4">
+        <v>0.06</v>
+      </c>
+      <c r="J4">
+        <v>-2788</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44715</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G5">
+        <v>4.2859999999999996</v>
+      </c>
+      <c r="H5">
+        <v>35.796999999999997</v>
+      </c>
+      <c r="I5">
+        <v>9.3420000000000005</v>
+      </c>
+      <c r="J5">
+        <v>442.92899999999997</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44715</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>3.19</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0.3</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>-872</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
         <v>44716</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>0.752</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>109.259</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>-1274.5909999999999</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44719</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>27.901</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>-908.08900000000006</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44719</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G9">
+        <v>3.996</v>
+      </c>
+      <c r="H9">
+        <v>36.936999999999998</v>
+      </c>
+      <c r="I9">
+        <v>10.484999999999999</v>
+      </c>
+      <c r="J9">
+        <v>461.476</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44725</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
         <v>21</v>
       </c>
-      <c r="D2">
-        <v>0.752</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>109.259</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>-1274.5909999999999</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>44715</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F10">
+        <v>1.9650000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>33.741</v>
+      </c>
+      <c r="I10">
+        <v>21.504000000000001</v>
+      </c>
+      <c r="J10">
+        <v>-1929.77</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B11" s="5">
+        <v>44725</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="D3">
-        <v>1.4E-2</v>
-      </c>
-      <c r="E3">
-        <v>4.2859999999999996</v>
-      </c>
-      <c r="F3">
-        <v>35.796999999999997</v>
-      </c>
-      <c r="G3">
-        <v>9.3420000000000005</v>
-      </c>
-      <c r="H3">
-        <v>442.92899999999997</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="F11">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>24.635999999999999</v>
+      </c>
+      <c r="I11">
+        <v>81.677000000000007</v>
+      </c>
+      <c r="J11">
+        <v>-1395.2660000000001</v>
+      </c>
+      <c r="K11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <v>44725</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1.931</v>
+      </c>
+      <c r="I12">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="J12">
+        <v>-1677.8810000000001</v>
+      </c>
+      <c r="K12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>44715</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4">
-        <v>3.19</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0.3</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>-136</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="B13" s="1">
+        <v>44726</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13">
+        <v>3.99</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>-2612.16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>44706</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5">
-        <v>0.34</v>
-      </c>
-      <c r="E5">
-        <v>3.67</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>6.99</v>
-      </c>
-      <c r="H5">
-        <v>313</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="B14" s="1">
+        <v>44726</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="G14">
+        <v>3.9510000000000001</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>3.9510000000000001</v>
+      </c>
+      <c r="J14">
+        <v>427.27499999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>44714</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>4.01</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>177</v>
-      </c>
-      <c r="G6">
-        <v>0.06</v>
-      </c>
-      <c r="H6">
-        <v>-2788</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="B15" s="1">
+        <v>44726</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G15">
+        <v>4.9960000000000004</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>4.9960000000000004</v>
+      </c>
+      <c r="J15">
+        <v>382.464</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>44719</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B16" s="5">
+        <v>44742</v>
+      </c>
+      <c r="C16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>27.901</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>-908.08900000000006</v>
-      </c>
-      <c r="I7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>44719</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="E8">
-        <v>3.996</v>
-      </c>
-      <c r="F8">
-        <v>36.936999999999998</v>
-      </c>
-      <c r="G8">
-        <v>10.484999999999999</v>
-      </c>
-      <c r="H8">
-        <v>461.476</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>44655</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>0.01</v>
-      </c>
-      <c r="E9">
-        <v>3.99</v>
-      </c>
-      <c r="F9">
-        <v>1.34</v>
-      </c>
-      <c r="G9">
-        <v>8.5399999999999991</v>
-      </c>
-      <c r="H9">
-        <v>487</v>
-      </c>
-      <c r="I9" t="s">
-        <v>25</v>
+      <c r="D16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K10">
+    <sortCondition ref="B1:B10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>